<commit_message>
commit as of 05/03/2020 -DB Doc Updated
</commit_message>
<xml_diff>
--- a/doc/TechRevamp/DBStructure.xlsx
+++ b/doc/TechRevamp/DBStructure.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kyobee11Nov\NewUI branch\RevisedKyobee\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kyobee11Nov\NewUI branch\RevisedKyobee\doc\TechRevamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="160">
   <si>
     <t>LOOKUP</t>
   </si>
@@ -366,6 +367,144 @@
   </si>
   <si>
     <t>BIGINT</t>
+  </si>
+  <si>
+    <t>BINARY</t>
+  </si>
+  <si>
+    <t>CHAR</t>
+  </si>
+  <si>
+    <t>Default - '1'</t>
+  </si>
+  <si>
+    <t>Default - 'Y'</t>
+  </si>
+  <si>
+    <t>Default - 'N'</t>
+  </si>
+  <si>
+    <t>ORGANIZATIONADCREDIT</t>
+  </si>
+  <si>
+    <t>OrganizationAdCreditID</t>
+  </si>
+  <si>
+    <t>CostPerAd</t>
+  </si>
+  <si>
+    <t>CurrencyID</t>
+  </si>
+  <si>
+    <t>NoOfAds</t>
+  </si>
+  <si>
+    <t>Transactiondate</t>
+  </si>
+  <si>
+    <t>TotalAmount</t>
+  </si>
+  <si>
+    <t>OrganizationPlanID</t>
+  </si>
+  <si>
+    <t>CreditType</t>
+  </si>
+  <si>
+    <t>ChargeID</t>
+  </si>
+  <si>
+    <t>DECIMAL</t>
+  </si>
+  <si>
+    <t>(10,2)</t>
+  </si>
+  <si>
+    <t>ORGANIZATIONLANG</t>
+  </si>
+  <si>
+    <t>This table is used to store language related to organization</t>
+  </si>
+  <si>
+    <t>OrganizationLangID</t>
+  </si>
+  <si>
+    <t>LanguageID</t>
+  </si>
+  <si>
+    <t>ORGANIZATIONCATEGORY</t>
+  </si>
+  <si>
+    <t>This table stores seating and marketing pref realted to organization</t>
+  </si>
+  <si>
+    <t>OrganizationCategoryID</t>
+  </si>
+  <si>
+    <t>CategoryTypeID</t>
+  </si>
+  <si>
+    <t>CategoryValueID</t>
+  </si>
+  <si>
+    <t>FK - ORGANIZATION Table</t>
+  </si>
+  <si>
+    <t>FK - LOOKUPTYPE Table</t>
+  </si>
+  <si>
+    <t>FK - LOOKUP Table</t>
+  </si>
+  <si>
+    <t>FK - LANGMASTER Table</t>
+  </si>
+  <si>
+    <t>ORGANIZATIONTEMPLATE</t>
+  </si>
+  <si>
+    <t>SmsTemplateID</t>
+  </si>
+  <si>
+    <t>This table stores information sms template related to organization</t>
+  </si>
+  <si>
+    <t>OrgID</t>
+  </si>
+  <si>
+    <t>TemplateText</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>ORGANIZATIONUSER</t>
+  </si>
+  <si>
+    <t>OrganizationUserID</t>
+  </si>
+  <si>
+    <t>This table is used to map user with organization</t>
+  </si>
+  <si>
+    <t>FK-ORGANIZATION Table</t>
+  </si>
+  <si>
+    <t>FK- USER Table</t>
+  </si>
+  <si>
+    <t>PLAN</t>
+  </si>
+  <si>
+    <t>This table is used to store plan related details</t>
+  </si>
+  <si>
+    <t>PlanID</t>
+  </si>
+  <si>
+    <t>PLANNAME</t>
+  </si>
+  <si>
+    <t>BIT</t>
   </si>
 </sst>
 </file>
@@ -389,7 +528,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,8 +547,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -566,11 +711,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -595,9 +760,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -610,6 +772,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -890,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J133"/>
+  <dimension ref="A1:J184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" topLeftCell="C166" workbookViewId="0">
+      <selection activeCell="G178" sqref="G178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,7 +1560,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="16" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="10"/>
@@ -1608,7 +1789,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="17" t="s">
         <v>39</v>
       </c>
       <c r="B37" s="14"/>
@@ -1856,7 +2037,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B50" s="14"/>
@@ -1866,7 +2047,7 @@
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
       <c r="H50" s="14"/>
-      <c r="I50" s="21"/>
+      <c r="I50" s="20"/>
       <c r="J50" s="14"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -2172,7 +2353,7 @@
       <c r="B66" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="C66" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D66" s="10">
@@ -2194,7 +2375,7 @@
       <c r="B67" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D67" s="11"/>
@@ -2241,7 +2422,7 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="18" t="s">
+      <c r="A70" s="17" t="s">
         <v>64</v>
       </c>
       <c r="B70" s="14"/>
@@ -2415,7 +2596,7 @@
       <c r="G79" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H79" s="22" t="s">
+      <c r="H79" s="21" t="s">
         <v>6</v>
       </c>
       <c r="I79" s="2" t="s">
@@ -2426,7 +2607,7 @@
       </c>
     </row>
     <row r="80" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
+      <c r="A80" s="16" t="s">
         <v>67</v>
       </c>
       <c r="B80" s="10"/>
@@ -2591,7 +2772,7 @@
       <c r="B89" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -2606,7 +2787,7 @@
       <c r="G89" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H89" s="22" t="s">
+      <c r="H89" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I89" s="2" t="s">
@@ -2620,326 +2801,2225 @@
       <c r="A90" s="16" t="s">
         <v>71</v>
       </c>
+      <c r="B90" s="10"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="10"/>
+      <c r="J90" s="10"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
+      <c r="A91" s="10"/>
+      <c r="B91" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="10">
         <v>11</v>
       </c>
-      <c r="E91" t="s">
-        <v>24</v>
-      </c>
-      <c r="F91" t="s">
-        <v>24</v>
-      </c>
-      <c r="G91" t="s">
-        <v>24</v>
-      </c>
+      <c r="E91" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F91" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G91" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H91" s="10"/>
+      <c r="I91" s="10"/>
+      <c r="J91" s="10"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
+      <c r="A92" s="10"/>
+      <c r="B92" s="10" t="s">
         <v>73</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="10">
         <v>255</v>
       </c>
-      <c r="F92" t="s">
-        <v>24</v>
-      </c>
+      <c r="E92" s="10"/>
+      <c r="F92" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G92" s="10"/>
+      <c r="H92" s="10"/>
+      <c r="I92" s="10"/>
+      <c r="J92" s="10"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
+      <c r="A93" s="10"/>
+      <c r="B93" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="10">
         <v>11</v>
       </c>
-      <c r="J93" t="s">
+      <c r="E93" s="10"/>
+      <c r="F93" s="10"/>
+      <c r="G93" s="10"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
+      <c r="J93" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+      <c r="A94" s="10"/>
+      <c r="B94" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="10">
         <v>11</v>
       </c>
-      <c r="F94" t="s">
-        <v>24</v>
-      </c>
+      <c r="E94" s="10"/>
+      <c r="F94" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G94" s="10"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10"/>
+      <c r="J94" s="10"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
+      <c r="A95" s="10"/>
+      <c r="B95" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="10">
         <v>11</v>
       </c>
-      <c r="J95" t="s">
+      <c r="E95" s="10"/>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10"/>
+      <c r="H95" s="10"/>
+      <c r="I95" s="10"/>
+      <c r="J95" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
+      <c r="A96" s="10"/>
+      <c r="B96" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="10">
         <v>11</v>
       </c>
-      <c r="F96" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
+      <c r="E96" s="10"/>
+      <c r="F96" s="10"/>
+      <c r="G96" s="10"/>
+      <c r="H96" s="10"/>
+      <c r="I96" s="10"/>
+      <c r="J96" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="10"/>
+      <c r="B97" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="10">
         <v>11</v>
       </c>
-      <c r="F97" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
+      <c r="E97" s="10"/>
+      <c r="F97" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+      <c r="J97" s="10"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="10"/>
+      <c r="B98" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="J98" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
+      <c r="C98" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D98" s="10">
+        <v>11</v>
+      </c>
+      <c r="E98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10"/>
+      <c r="H98" s="10"/>
+      <c r="I98" s="10"/>
+      <c r="J98" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="10"/>
+      <c r="B99" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="F99" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
+      <c r="C99" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D99" s="10">
+        <v>255</v>
+      </c>
+      <c r="E99" s="10"/>
+      <c r="F99" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G99" s="10"/>
+      <c r="H99" s="10"/>
+      <c r="I99" s="10"/>
+      <c r="J99" s="10"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="10"/>
+      <c r="B100" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="J100" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
+      <c r="C100" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D100" s="10">
+        <v>255</v>
+      </c>
+      <c r="E100" s="10"/>
+      <c r="F100" s="10"/>
+      <c r="G100" s="10"/>
+      <c r="H100" s="10"/>
+      <c r="I100" s="10"/>
+      <c r="J100" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="10"/>
+      <c r="B101" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="J101" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
+      <c r="C101" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D101" s="10">
+        <v>1</v>
+      </c>
+      <c r="E101" s="10"/>
+      <c r="F101" s="10"/>
+      <c r="G101" s="10"/>
+      <c r="H101" s="10"/>
+      <c r="I101" s="10"/>
+      <c r="J101" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="10"/>
+      <c r="B102" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="J102" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
+      <c r="C102" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D102" s="10">
+        <v>1</v>
+      </c>
+      <c r="E102" s="10"/>
+      <c r="F102" s="10"/>
+      <c r="G102" s="10"/>
+      <c r="H102" s="10"/>
+      <c r="I102" s="10"/>
+      <c r="J102" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="10"/>
+      <c r="B103" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="J103" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
+      <c r="C103" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D103" s="10">
+        <v>1</v>
+      </c>
+      <c r="E103" s="10"/>
+      <c r="F103" s="10"/>
+      <c r="G103" s="10"/>
+      <c r="H103" s="10"/>
+      <c r="I103" s="10"/>
+      <c r="J103" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="10"/>
+      <c r="B104" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="J104" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
+      <c r="C104" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D104" s="10">
+        <v>1</v>
+      </c>
+      <c r="E104" s="10"/>
+      <c r="F104" s="10"/>
+      <c r="G104" s="10"/>
+      <c r="H104" s="10"/>
+      <c r="I104" s="10"/>
+      <c r="J104" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="10"/>
+      <c r="B105" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="J105" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
+      <c r="C105" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D105" s="10">
+        <v>255</v>
+      </c>
+      <c r="E105" s="10"/>
+      <c r="F105" s="10"/>
+      <c r="G105" s="10"/>
+      <c r="H105" s="10"/>
+      <c r="I105" s="10"/>
+      <c r="J105" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="10"/>
+      <c r="B106" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J106" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
+      <c r="C106" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D106" s="10">
+        <v>255</v>
+      </c>
+      <c r="E106" s="10"/>
+      <c r="F106" s="10"/>
+      <c r="G106" s="10"/>
+      <c r="H106" s="10"/>
+      <c r="I106" s="10"/>
+      <c r="J106" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="10"/>
+      <c r="B107" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="J107" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
+      <c r="C107" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D107" s="10">
+        <v>11</v>
+      </c>
+      <c r="E107" s="10"/>
+      <c r="F107" s="10"/>
+      <c r="G107" s="10"/>
+      <c r="H107" s="10"/>
+      <c r="I107" s="10"/>
+      <c r="J107" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="10"/>
+      <c r="B108" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="J108" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
+      <c r="C108" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D108" s="10">
+        <v>11</v>
+      </c>
+      <c r="E108" s="10"/>
+      <c r="F108" s="10"/>
+      <c r="G108" s="10"/>
+      <c r="H108" s="10"/>
+      <c r="I108" s="10"/>
+      <c r="J108" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="10"/>
+      <c r="B109" s="23" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
+      <c r="C109" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D109" s="10">
+        <v>1</v>
+      </c>
+      <c r="E109" s="10"/>
+      <c r="F109" s="10"/>
+      <c r="G109" s="10"/>
+      <c r="H109" s="10"/>
+      <c r="I109" s="10"/>
+      <c r="J109" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="10"/>
+      <c r="B110" s="23" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
+      <c r="C110" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D110" s="10">
+        <v>50</v>
+      </c>
+      <c r="E110" s="10"/>
+      <c r="F110" s="10"/>
+      <c r="G110" s="10"/>
+      <c r="H110" s="10"/>
+      <c r="I110" s="10"/>
+      <c r="J110" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="10"/>
+      <c r="B111" s="23" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B112" t="s">
+      <c r="C111" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D111" s="10">
+        <v>100</v>
+      </c>
+      <c r="E111" s="10"/>
+      <c r="F111" s="10"/>
+      <c r="G111" s="10"/>
+      <c r="H111" s="10"/>
+      <c r="I111" s="10"/>
+      <c r="J111" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="10"/>
+      <c r="B112" s="23" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
+      <c r="C112" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D112" s="10">
+        <v>1</v>
+      </c>
+      <c r="E112" s="10"/>
+      <c r="F112" s="10"/>
+      <c r="G112" s="10"/>
+      <c r="H112" s="10"/>
+      <c r="I112" s="10"/>
+      <c r="J112" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="10"/>
+      <c r="B113" s="23" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
+      <c r="C113" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D113" s="10">
+        <v>255</v>
+      </c>
+      <c r="E113" s="10"/>
+      <c r="F113" s="10"/>
+      <c r="G113" s="10"/>
+      <c r="H113" s="10"/>
+      <c r="I113" s="10"/>
+      <c r="J113" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="10"/>
+      <c r="B114" s="23" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
+      <c r="C114" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D114" s="10">
+        <v>2000</v>
+      </c>
+      <c r="E114" s="10"/>
+      <c r="F114" s="10"/>
+      <c r="G114" s="10"/>
+      <c r="H114" s="10"/>
+      <c r="I114" s="10"/>
+      <c r="J114" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="10"/>
+      <c r="B115" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" t="s">
+      <c r="C115" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D115" s="10">
+        <v>1</v>
+      </c>
+      <c r="E115" s="10"/>
+      <c r="F115" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G115" s="10"/>
+      <c r="H115" s="10"/>
+      <c r="I115" s="10"/>
+      <c r="J115" s="10"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" s="10"/>
+      <c r="B116" s="10" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" t="s">
+      <c r="C116" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D116" s="10">
+        <v>11</v>
+      </c>
+      <c r="E116" s="10"/>
+      <c r="F116" s="10"/>
+      <c r="G116" s="10"/>
+      <c r="H116" s="10"/>
+      <c r="I116" s="10"/>
+      <c r="J116" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" s="10"/>
+      <c r="B117" s="10" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" t="s">
+      <c r="C117" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D117" s="10">
+        <v>11</v>
+      </c>
+      <c r="E117" s="10"/>
+      <c r="F117" s="10"/>
+      <c r="G117" s="10"/>
+      <c r="H117" s="10"/>
+      <c r="I117" s="10"/>
+      <c r="J117" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118" s="10"/>
+      <c r="B118" s="10" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" t="s">
+      <c r="C118" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D118" s="10">
+        <v>50</v>
+      </c>
+      <c r="E118" s="10"/>
+      <c r="F118" s="10"/>
+      <c r="G118" s="10"/>
+      <c r="H118" s="10"/>
+      <c r="I118" s="10"/>
+      <c r="J118" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" s="10"/>
+      <c r="B119" s="10" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" t="s">
+      <c r="C119" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D119" s="10">
+        <v>255</v>
+      </c>
+      <c r="E119" s="10"/>
+      <c r="F119" s="10"/>
+      <c r="G119" s="10"/>
+      <c r="H119" s="10"/>
+      <c r="I119" s="10"/>
+      <c r="J119" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120" s="10"/>
+      <c r="B120" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" t="s">
+      <c r="C120" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D120" s="10">
+        <v>100</v>
+      </c>
+      <c r="E120" s="10"/>
+      <c r="F120" s="10"/>
+      <c r="G120" s="10"/>
+      <c r="H120" s="10"/>
+      <c r="I120" s="10"/>
+      <c r="J120" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A121" s="10"/>
+      <c r="B121" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" t="s">
+      <c r="C121" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
+      <c r="F121" s="10"/>
+      <c r="G121" s="10"/>
+      <c r="H121" s="10"/>
+      <c r="I121" s="10"/>
+      <c r="J121" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A122" s="10"/>
+      <c r="B122" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
+      <c r="C122" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D122" s="10">
+        <v>100</v>
+      </c>
+      <c r="E122" s="10"/>
+      <c r="F122" s="10"/>
+      <c r="G122" s="10"/>
+      <c r="H122" s="10"/>
+      <c r="I122" s="10"/>
+      <c r="J122" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A123" s="10"/>
+      <c r="B123" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" t="s">
+      <c r="C123" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="10"/>
+      <c r="G123" s="10"/>
+      <c r="H123" s="10"/>
+      <c r="I123" s="10"/>
+      <c r="J123" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A124" s="10"/>
+      <c r="B124" s="10" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" t="s">
+      <c r="C124" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D124" s="10">
+        <v>10</v>
+      </c>
+      <c r="E124" s="10"/>
+      <c r="F124" s="10"/>
+      <c r="G124" s="10"/>
+      <c r="H124" s="10"/>
+      <c r="I124" s="10"/>
+      <c r="J124" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A125" s="10"/>
+      <c r="B125" s="10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" t="s">
+      <c r="C125" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D125" s="10">
+        <v>100</v>
+      </c>
+      <c r="E125" s="10"/>
+      <c r="F125" s="10"/>
+      <c r="G125" s="10"/>
+      <c r="H125" s="10"/>
+      <c r="I125" s="10"/>
+      <c r="J125" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A126" s="10"/>
+      <c r="B126" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" t="s">
+      <c r="C126" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D126" s="10">
+        <v>100</v>
+      </c>
+      <c r="E126" s="10"/>
+      <c r="F126" s="10"/>
+      <c r="G126" s="10"/>
+      <c r="H126" s="10"/>
+      <c r="I126" s="10"/>
+      <c r="J126" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A127" s="10"/>
+      <c r="B127" s="23" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" t="s">
+      <c r="C127" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D127" s="10">
+        <v>255</v>
+      </c>
+      <c r="E127" s="10"/>
+      <c r="F127" s="10"/>
+      <c r="G127" s="10"/>
+      <c r="H127" s="10"/>
+      <c r="I127" s="10"/>
+      <c r="J127" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A128" s="10"/>
+      <c r="B128" s="10" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" t="s">
+      <c r="C128" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D128" s="10">
+        <v>45</v>
+      </c>
+      <c r="E128" s="10"/>
+      <c r="F128" s="10"/>
+      <c r="G128" s="10"/>
+      <c r="H128" s="10"/>
+      <c r="I128" s="10"/>
+      <c r="J128" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A129" s="10"/>
+      <c r="B129" s="10" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" t="s">
+      <c r="C129" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D129" s="10">
+        <v>1</v>
+      </c>
+      <c r="E129" s="10"/>
+      <c r="F129" s="10"/>
+      <c r="G129" s="10"/>
+      <c r="H129" s="10"/>
+      <c r="I129" s="10"/>
+      <c r="J129" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A130" s="10"/>
+      <c r="B130" s="10" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
+      <c r="C130" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D130" s="10">
+        <v>1</v>
+      </c>
+      <c r="E130" s="10"/>
+      <c r="F130" s="10"/>
+      <c r="G130" s="10"/>
+      <c r="H130" s="10"/>
+      <c r="I130" s="10"/>
+      <c r="J130" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131" s="10"/>
+      <c r="B131" s="10" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" t="s">
+      <c r="C131" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D131" s="10">
+        <v>300</v>
+      </c>
+      <c r="E131" s="10"/>
+      <c r="F131" s="10"/>
+      <c r="G131" s="10"/>
+      <c r="H131" s="10"/>
+      <c r="I131" s="10"/>
+      <c r="J131" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A132" s="10"/>
+      <c r="B132" s="10" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" t="s">
+      <c r="C132" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D132" s="10">
+        <v>10</v>
+      </c>
+      <c r="E132" s="10"/>
+      <c r="F132" s="10"/>
+      <c r="G132" s="10"/>
+      <c r="H132" s="10"/>
+      <c r="I132" s="10"/>
+      <c r="J132" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="11"/>
+      <c r="B133" s="11" t="s">
         <v>112</v>
       </c>
+      <c r="C133" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D133" s="11">
+        <v>10</v>
+      </c>
+      <c r="E133" s="11"/>
+      <c r="F133" s="11"/>
+      <c r="G133" s="11"/>
+      <c r="H133" s="11"/>
+      <c r="I133" s="11"/>
+      <c r="J133" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="135" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B135" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H135" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I135" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J135" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A136" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B136" s="10"/>
+      <c r="C136" s="10"/>
+      <c r="D136" s="10"/>
+      <c r="E136" s="10"/>
+      <c r="F136" s="10"/>
+      <c r="G136" s="10"/>
+      <c r="H136" s="5"/>
+      <c r="I136" s="14"/>
+      <c r="J136" s="6"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137" s="4"/>
+      <c r="B137" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C137" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D137" s="10">
+        <v>11</v>
+      </c>
+      <c r="E137" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F137" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G137" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H137" s="5"/>
+      <c r="I137" s="10"/>
+      <c r="J137" s="6"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138" s="4"/>
+      <c r="B138" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C138" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D138" s="10">
+        <v>11</v>
+      </c>
+      <c r="E138" s="10"/>
+      <c r="F138" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G138" s="10"/>
+      <c r="H138" s="5"/>
+      <c r="I138" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J138" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139" s="4"/>
+      <c r="B139" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C139" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D139" s="10">
+        <v>11</v>
+      </c>
+      <c r="E139" s="10"/>
+      <c r="F139" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G139" s="10"/>
+      <c r="H139" s="5"/>
+      <c r="I139" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J139" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A140" s="4"/>
+      <c r="B140" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C140" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D140" s="10">
+        <v>1</v>
+      </c>
+      <c r="E140" s="10"/>
+      <c r="F140" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G140" s="10"/>
+      <c r="H140" s="5"/>
+      <c r="I140" s="10"/>
+      <c r="J140" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A141" s="4"/>
+      <c r="B141" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C141" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D141" s="10">
+        <v>100</v>
+      </c>
+      <c r="E141" s="10"/>
+      <c r="F141" s="10"/>
+      <c r="G141" s="10"/>
+      <c r="H141" s="5"/>
+      <c r="I141" s="10"/>
+      <c r="J141" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A142" s="4"/>
+      <c r="B142" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C142" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D142" s="10"/>
+      <c r="E142" s="10"/>
+      <c r="F142" s="10"/>
+      <c r="G142" s="10"/>
+      <c r="H142" s="5"/>
+      <c r="I142" s="10"/>
+      <c r="J142" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143" s="4"/>
+      <c r="B143" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C143" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D143" s="10">
+        <v>100</v>
+      </c>
+      <c r="E143" s="10"/>
+      <c r="F143" s="10"/>
+      <c r="G143" s="10"/>
+      <c r="H143" s="5"/>
+      <c r="I143" s="10"/>
+      <c r="J143" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="7"/>
+      <c r="B144" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C144" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D144" s="11"/>
+      <c r="E144" s="11"/>
+      <c r="F144" s="11"/>
+      <c r="G144" s="11"/>
+      <c r="H144" s="8"/>
+      <c r="I144" s="11"/>
+      <c r="J144" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="146" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B146" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D146" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H146" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I146" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J146" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A147" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B147" s="10"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="6"/>
+      <c r="E147" s="10"/>
+      <c r="F147" s="10"/>
+      <c r="G147" s="10"/>
+      <c r="H147" s="10"/>
+      <c r="I147" s="10"/>
+      <c r="J147" s="10"/>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A148" s="4"/>
+      <c r="B148" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C148" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D148" s="6">
+        <v>11</v>
+      </c>
+      <c r="E148" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F148" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G148" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H148" s="10"/>
+      <c r="I148" s="10"/>
+      <c r="J148" s="10"/>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A149" s="4"/>
+      <c r="B149" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C149" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D149" s="6">
+        <v>11</v>
+      </c>
+      <c r="E149" s="10"/>
+      <c r="F149" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G149" s="10"/>
+      <c r="H149" s="10"/>
+      <c r="I149" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J149" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A150" s="4"/>
+      <c r="B150" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C150" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D150" s="6">
+        <v>11</v>
+      </c>
+      <c r="E150" s="10"/>
+      <c r="F150" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G150" s="10"/>
+      <c r="H150" s="10"/>
+      <c r="I150" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J150" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="7"/>
+      <c r="B151" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C151" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D151" s="9">
+        <v>11</v>
+      </c>
+      <c r="E151" s="11"/>
+      <c r="F151" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G151" s="11"/>
+      <c r="H151" s="11"/>
+      <c r="I151" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J151" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="153" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B153" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D153" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H153" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I153" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J153" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A154" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B154" s="14"/>
+      <c r="D154" s="14"/>
+      <c r="E154" s="14"/>
+      <c r="F154" s="14"/>
+      <c r="G154" s="14"/>
+      <c r="H154" s="14"/>
+      <c r="I154" s="14"/>
+      <c r="J154" s="14"/>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A155" s="10"/>
+      <c r="B155" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C155" t="s">
+        <v>22</v>
+      </c>
+      <c r="D155" s="10">
+        <v>11</v>
+      </c>
+      <c r="E155" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F155" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G155" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H155" s="10"/>
+      <c r="I155" s="10"/>
+      <c r="J155" s="10"/>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A156" s="10"/>
+      <c r="B156" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C156" t="s">
+        <v>22</v>
+      </c>
+      <c r="D156" s="10">
+        <v>11</v>
+      </c>
+      <c r="E156" s="10"/>
+      <c r="F156" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G156" s="10"/>
+      <c r="H156" s="10"/>
+      <c r="I156" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J156" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A157" s="10"/>
+      <c r="B157" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C157" t="s">
+        <v>22</v>
+      </c>
+      <c r="D157" s="10">
+        <v>11</v>
+      </c>
+      <c r="E157" s="10"/>
+      <c r="F157" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G157" s="10"/>
+      <c r="H157" s="10"/>
+      <c r="I157" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J157" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A158" s="10"/>
+      <c r="B158" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C158" t="s">
+        <v>23</v>
+      </c>
+      <c r="D158" s="10">
+        <v>250</v>
+      </c>
+      <c r="E158" s="10"/>
+      <c r="F158" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G158" s="10"/>
+      <c r="H158" s="10"/>
+      <c r="I158" s="10"/>
+      <c r="J158" s="10"/>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A159" s="10"/>
+      <c r="B159" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C159" t="s">
+        <v>22</v>
+      </c>
+      <c r="D159" s="10">
+        <v>11</v>
+      </c>
+      <c r="E159" s="10"/>
+      <c r="F159" s="10"/>
+      <c r="G159" s="10"/>
+      <c r="H159" s="10"/>
+      <c r="I159" s="10"/>
+      <c r="J159" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A160" s="10"/>
+      <c r="B160" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C160" t="s">
+        <v>36</v>
+      </c>
+      <c r="D160" s="10">
+        <v>1</v>
+      </c>
+      <c r="E160" s="10"/>
+      <c r="F160" s="10"/>
+      <c r="G160" s="10"/>
+      <c r="H160" s="10"/>
+      <c r="I160" s="10"/>
+      <c r="J160" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A161" s="10"/>
+      <c r="B161" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D161" s="10">
+        <v>100</v>
+      </c>
+      <c r="E161" s="10"/>
+      <c r="F161" s="10"/>
+      <c r="G161" s="10"/>
+      <c r="H161" s="10"/>
+      <c r="I161" s="10"/>
+      <c r="J161" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A162" s="10"/>
+      <c r="B162" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D162" s="10"/>
+      <c r="E162" s="10"/>
+      <c r="F162" s="10"/>
+      <c r="G162" s="10"/>
+      <c r="H162" s="10"/>
+      <c r="I162" s="10"/>
+      <c r="J162" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163" s="10"/>
+      <c r="B163" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D163" s="10">
+        <v>100</v>
+      </c>
+      <c r="E163" s="10"/>
+      <c r="F163" s="10"/>
+      <c r="G163" s="10"/>
+      <c r="H163" s="10"/>
+      <c r="I163" s="10"/>
+      <c r="J163" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="11"/>
+      <c r="B164" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C164" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D164" s="11"/>
+      <c r="E164" s="11"/>
+      <c r="F164" s="11"/>
+      <c r="G164" s="11"/>
+      <c r="H164" s="11"/>
+      <c r="I164" s="11"/>
+      <c r="J164" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="166" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B166" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C166" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E166" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G166" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I166" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J166" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A167" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B167" s="14"/>
+      <c r="C167" s="30"/>
+      <c r="D167" s="14"/>
+      <c r="E167" s="30"/>
+      <c r="F167" s="14"/>
+      <c r="G167" s="30"/>
+      <c r="H167" s="14"/>
+      <c r="I167" s="14"/>
+      <c r="J167" s="31"/>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A168" s="4"/>
+      <c r="B168" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D168" s="10">
+        <v>11</v>
+      </c>
+      <c r="E168" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F168" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G168" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H168" s="10"/>
+      <c r="I168" s="10"/>
+      <c r="J168" s="6"/>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A169" s="4"/>
+      <c r="B169" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C169" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D169" s="10">
+        <v>11</v>
+      </c>
+      <c r="E169" s="5"/>
+      <c r="F169" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G169" s="5"/>
+      <c r="H169" s="10"/>
+      <c r="I169" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J169" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A170" s="4"/>
+      <c r="B170" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C170" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D170" s="10">
+        <v>11</v>
+      </c>
+      <c r="E170" s="5"/>
+      <c r="F170" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G170" s="5"/>
+      <c r="H170" s="10"/>
+      <c r="I170" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J170" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A171" s="4"/>
+      <c r="B171" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C171" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D171" s="10">
+        <v>100</v>
+      </c>
+      <c r="E171" s="5"/>
+      <c r="F171" s="10"/>
+      <c r="G171" s="5"/>
+      <c r="H171" s="10"/>
+      <c r="I171" s="10"/>
+      <c r="J171" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A172" s="4"/>
+      <c r="B172" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C172" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D172" s="10"/>
+      <c r="E172" s="5"/>
+      <c r="F172" s="10"/>
+      <c r="G172" s="5"/>
+      <c r="H172" s="10"/>
+      <c r="I172" s="10"/>
+      <c r="J172" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A173" s="4"/>
+      <c r="B173" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C173" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D173" s="10">
+        <v>100</v>
+      </c>
+      <c r="E173" s="5"/>
+      <c r="F173" s="10"/>
+      <c r="G173" s="5"/>
+      <c r="H173" s="10"/>
+      <c r="I173" s="10"/>
+      <c r="J173" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="7"/>
+      <c r="B174" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C174" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D174" s="11"/>
+      <c r="E174" s="8"/>
+      <c r="F174" s="11"/>
+      <c r="G174" s="8"/>
+      <c r="H174" s="11"/>
+      <c r="I174" s="11"/>
+      <c r="J174" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="176" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B176" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C176" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E176" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G176" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H176" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I176" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J176" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A177" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B177" s="10"/>
+      <c r="C177" s="5"/>
+      <c r="D177" s="10"/>
+      <c r="E177" s="5"/>
+      <c r="F177" s="10"/>
+      <c r="G177" s="5"/>
+      <c r="H177" s="10"/>
+      <c r="I177" s="10"/>
+      <c r="J177" s="6"/>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A178" s="4"/>
+      <c r="B178" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C178" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D178" s="10">
+        <v>11</v>
+      </c>
+      <c r="E178" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F178" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G178" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H178" s="10"/>
+      <c r="I178" s="10"/>
+      <c r="J178" s="6"/>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A179" s="4"/>
+      <c r="B179" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C179" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D179" s="10">
+        <v>80</v>
+      </c>
+      <c r="E179" s="5"/>
+      <c r="F179" s="10"/>
+      <c r="G179" s="5"/>
+      <c r="H179" s="10"/>
+      <c r="I179" s="10"/>
+      <c r="J179" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A180" s="4"/>
+      <c r="B180" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C180" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D180" s="10">
+        <v>100</v>
+      </c>
+      <c r="E180" s="5"/>
+      <c r="F180" s="10"/>
+      <c r="G180" s="5"/>
+      <c r="H180" s="10"/>
+      <c r="I180" s="10"/>
+      <c r="J180" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A181" s="4"/>
+      <c r="B181" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C181" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D181" s="10"/>
+      <c r="E181" s="5"/>
+      <c r="F181" s="10"/>
+      <c r="G181" s="5"/>
+      <c r="H181" s="10"/>
+      <c r="I181" s="10"/>
+      <c r="J181" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A182" s="4"/>
+      <c r="B182" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C182" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D182" s="10">
+        <v>100</v>
+      </c>
+      <c r="E182" s="5"/>
+      <c r="F182" s="10"/>
+      <c r="G182" s="5"/>
+      <c r="H182" s="10"/>
+      <c r="I182" s="10"/>
+      <c r="J182" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A183" s="4"/>
+      <c r="B183" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C183" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D183" s="10"/>
+      <c r="E183" s="5"/>
+      <c r="F183" s="10"/>
+      <c r="G183" s="5"/>
+      <c r="H183" s="10"/>
+      <c r="I183" s="10"/>
+      <c r="J183" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="7"/>
+      <c r="B184" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C184" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="D184" s="11">
+        <v>1</v>
+      </c>
+      <c r="E184" s="8"/>
+      <c r="F184" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G184" s="8"/>
+      <c r="H184" s="11"/>
+      <c r="I184" s="11"/>
+      <c r="J184" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="10">
+        <v>11</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="10">
+        <v>11</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="10">
+        <v>11</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="10">
+        <v>11</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="10">
+        <v>11</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="10">
+        <v>11</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="10">
+        <v>100</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="10">
+        <v>100</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="11">
+        <v>255</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- commited for db structure file
</commit_message>
<xml_diff>
--- a/doc/TechRevamp/DBStructure.xlsx
+++ b/doc/TechRevamp/DBStructure.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kyobee11Nov\NewUI branch\RevisedKyobee\doc\TechRevamp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ria\Kyobee\Kyobee\RevisedKyobee\doc\TechRevamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="234">
   <si>
     <t>LOOKUP</t>
   </si>
@@ -505,12 +505,234 @@
   </si>
   <si>
     <t>BIT</t>
+  </si>
+  <si>
+    <t>ORGANIZATIONTYPE</t>
+  </si>
+  <si>
+    <t>This table stores details of organization type</t>
+  </si>
+  <si>
+    <t>TypeId</t>
+  </si>
+  <si>
+    <t>TypeName</t>
+  </si>
+  <si>
+    <t>GUEST</t>
+  </si>
+  <si>
+    <t>This table is used to store guest details</t>
+  </si>
+  <si>
+    <t>guestID</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t>noOfChildren</t>
+  </si>
+  <si>
+    <t>noOfAdults</t>
+  </si>
+  <si>
+    <t>noOfInfants</t>
+  </si>
+  <si>
+    <t>noOfPeople</t>
+  </si>
+  <si>
+    <t>quoteTime</t>
+  </si>
+  <si>
+    <t>partyType</t>
+  </si>
+  <si>
+    <t>Default - -1</t>
+  </si>
+  <si>
+    <t>deviceType</t>
+  </si>
+  <si>
+    <t>deviceId</t>
+  </si>
+  <si>
+    <t>contactNo</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>prefType</t>
+  </si>
+  <si>
+    <t>languagePrefID</t>
+  </si>
+  <si>
+    <t>optin</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>seatingPreference</t>
+  </si>
+  <si>
+    <t>recvLeveltwo</t>
+  </si>
+  <si>
+    <t>calloutCount</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>incompleteParty</t>
+  </si>
+  <si>
+    <t>resetTime</t>
+  </si>
+  <si>
+    <t>checkinTime</t>
+  </si>
+  <si>
+    <t>seatedTime</t>
+  </si>
+  <si>
+    <t>createdTime</t>
+  </si>
+  <si>
+    <t>updatedTime</t>
+  </si>
+  <si>
+    <t>marketingPreference</t>
+  </si>
+  <si>
+    <t>GUESTRESET</t>
+  </si>
+  <si>
+    <t>This table is used to store guest details reset by organization</t>
+  </si>
+  <si>
+    <t>guestResetID</t>
+  </si>
+  <si>
+    <t>GUESTMARKETINGPREFERENCES</t>
+  </si>
+  <si>
+    <t>This table stores marketing pref realted to guest</t>
+  </si>
+  <si>
+    <t>GUEST_MARKETING_PREF_ID</t>
+  </si>
+  <si>
+    <t>PREF_ID</t>
+  </si>
+  <si>
+    <t>GUEST_ID</t>
+  </si>
+  <si>
+    <t>FK - GUEST Table</t>
+  </si>
+  <si>
+    <t>GUESTMARKETINGPREFERENCESRESET</t>
+  </si>
+  <si>
+    <t>This table stores guest marketing pref details reset by organization</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>AddressLineOne</t>
+  </si>
+  <si>
+    <t>AddressLineTwo</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>ActiveFlag</t>
+  </si>
+  <si>
+    <t>10,6</t>
+  </si>
+  <si>
+    <t>DEFAULT - 0</t>
+  </si>
+  <si>
+    <t>SmsLogID</t>
+  </si>
+  <si>
+    <t>TemplateID</t>
+  </si>
+  <si>
+    <t>TemplateLevel</t>
+  </si>
+  <si>
+    <t>GuestID</t>
+  </si>
+  <si>
+    <t>PhoneNo</t>
+  </si>
+  <si>
+    <t>MessageText</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>This table stores address of user</t>
+  </si>
+  <si>
+    <t>SMSLOG</t>
+  </si>
+  <si>
+    <t>SMSTEMPLATELANGUAGEMAPPING</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IsoCode</t>
+  </si>
+  <si>
+    <t>This table stores sms template related of all languages</t>
+  </si>
+  <si>
+    <t>This table stores logs of all sms send to user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -528,7 +750,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -550,6 +772,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,7 +963,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -775,7 +1003,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -791,6 +1018,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1071,16 +1308,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J184"/>
+  <dimension ref="A1:J317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C166" workbookViewId="0">
-      <selection activeCell="G178" sqref="G178"/>
+    <sheetView tabSelected="1" topLeftCell="A314" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="23.85546875" customWidth="1"/>
@@ -2997,7 +3234,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="10"/>
-      <c r="B100" s="23" t="s">
+      <c r="B100" s="36" t="s">
         <v>83</v>
       </c>
       <c r="C100" s="10" t="s">
@@ -3017,7 +3254,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="10"/>
-      <c r="B101" s="23" t="s">
+      <c r="B101" s="36" t="s">
         <v>84</v>
       </c>
       <c r="C101" s="18" t="s">
@@ -3037,7 +3274,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="10"/>
-      <c r="B102" s="23" t="s">
+      <c r="B102" s="36" t="s">
         <v>85</v>
       </c>
       <c r="C102" s="18" t="s">
@@ -3057,7 +3294,7 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="10"/>
-      <c r="B103" s="23" t="s">
+      <c r="B103" s="36" t="s">
         <v>86</v>
       </c>
       <c r="C103" s="18" t="s">
@@ -3077,7 +3314,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="10"/>
-      <c r="B104" s="23" t="s">
+      <c r="B104" s="36" t="s">
         <v>87</v>
       </c>
       <c r="C104" s="18" t="s">
@@ -3097,7 +3334,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="10"/>
-      <c r="B105" s="23" t="s">
+      <c r="B105" s="36" t="s">
         <v>88</v>
       </c>
       <c r="C105" s="10" t="s">
@@ -3117,7 +3354,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="10"/>
-      <c r="B106" s="23" t="s">
+      <c r="B106" s="36" t="s">
         <v>89</v>
       </c>
       <c r="C106" s="10" t="s">
@@ -3137,7 +3374,7 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="10"/>
-      <c r="B107" s="23" t="s">
+      <c r="B107" s="36" t="s">
         <v>90</v>
       </c>
       <c r="C107" s="10" t="s">
@@ -3157,7 +3394,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="10"/>
-      <c r="B108" s="23" t="s">
+      <c r="B108" s="36" t="s">
         <v>91</v>
       </c>
       <c r="C108" s="10" t="s">
@@ -3177,7 +3414,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="10"/>
-      <c r="B109" s="23" t="s">
+      <c r="B109" s="36" t="s">
         <v>92</v>
       </c>
       <c r="C109" s="10" t="s">
@@ -3197,7 +3434,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="10"/>
-      <c r="B110" s="23" t="s">
+      <c r="B110" s="36" t="s">
         <v>93</v>
       </c>
       <c r="C110" s="10" t="s">
@@ -3217,7 +3454,7 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="10"/>
-      <c r="B111" s="23" t="s">
+      <c r="B111" s="36" t="s">
         <v>94</v>
       </c>
       <c r="C111" s="10" t="s">
@@ -3237,7 +3474,7 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="10"/>
-      <c r="B112" s="23" t="s">
+      <c r="B112" s="37" t="s">
         <v>95</v>
       </c>
       <c r="C112" s="10" t="s">
@@ -3257,7 +3494,7 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="10"/>
-      <c r="B113" s="23" t="s">
+      <c r="B113" s="37" t="s">
         <v>96</v>
       </c>
       <c r="C113" s="10" t="s">
@@ -3277,7 +3514,7 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
-      <c r="B114" s="23" t="s">
+      <c r="B114" s="36" t="s">
         <v>97</v>
       </c>
       <c r="C114" s="10" t="s">
@@ -3513,7 +3750,7 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="10"/>
-      <c r="B126" s="10" t="s">
+      <c r="B126" s="37" t="s">
         <v>105</v>
       </c>
       <c r="C126" s="18" t="s">
@@ -3533,7 +3770,7 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="10"/>
-      <c r="B127" s="23" t="s">
+      <c r="B127" s="36" t="s">
         <v>106</v>
       </c>
       <c r="C127" s="18" t="s">
@@ -3553,7 +3790,7 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="10"/>
-      <c r="B128" s="10" t="s">
+      <c r="B128" s="37" t="s">
         <v>107</v>
       </c>
       <c r="C128" s="18" t="s">
@@ -3593,7 +3830,7 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="10"/>
-      <c r="B130" s="10" t="s">
+      <c r="B130" s="37" t="s">
         <v>109</v>
       </c>
       <c r="C130" s="18" t="s">
@@ -3613,7 +3850,7 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="10"/>
-      <c r="B131" s="10" t="s">
+      <c r="B131" s="37" t="s">
         <v>110</v>
       </c>
       <c r="C131" s="18" t="s">
@@ -3676,7 +3913,7 @@
       <c r="A135" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B135" s="24" t="s">
+      <c r="B135" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C135" s="1" t="s">
@@ -3893,7 +4130,7 @@
       <c r="A146" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B146" s="24" t="s">
+      <c r="B146" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C146" s="1" t="s">
@@ -4036,7 +4273,7 @@
       <c r="A153" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B153" s="24" t="s">
+      <c r="B153" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C153" s="1" t="s">
@@ -4290,10 +4527,10 @@
       <c r="A166" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="B166" s="24" t="s">
+      <c r="B166" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C166" s="28" t="s">
+      <c r="C166" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D166" s="1" t="s">
@@ -4319,18 +4556,18 @@
       </c>
     </row>
     <row r="167" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="29" t="s">
+      <c r="A167" s="28" t="s">
         <v>152</v>
       </c>
       <c r="B167" s="14"/>
-      <c r="C167" s="30"/>
+      <c r="C167" s="29"/>
       <c r="D167" s="14"/>
-      <c r="E167" s="30"/>
+      <c r="E167" s="29"/>
       <c r="F167" s="14"/>
-      <c r="G167" s="30"/>
+      <c r="G167" s="29"/>
       <c r="H167" s="14"/>
       <c r="I167" s="14"/>
-      <c r="J167" s="31"/>
+      <c r="J167" s="30"/>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="4"/>
@@ -4485,7 +4722,7 @@
       <c r="A176" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="B176" s="24" t="s">
+      <c r="B176" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C176" s="21" t="s">
@@ -4652,7 +4889,7 @@
       <c r="B184" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C184" s="32" t="s">
+      <c r="C184" s="31" t="s">
         <v>159</v>
       </c>
       <c r="D184" s="11">
@@ -4666,6 +4903,2540 @@
       <c r="H184" s="11"/>
       <c r="I184" s="11"/>
       <c r="J184" s="9"/>
+    </row>
+    <row r="185" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="186" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H186" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I186" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J186" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A187" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B187" s="14"/>
+      <c r="C187" s="14"/>
+      <c r="D187" s="14"/>
+      <c r="E187" s="14"/>
+      <c r="F187" s="14"/>
+      <c r="G187" s="14"/>
+      <c r="H187" s="14"/>
+      <c r="I187" s="14"/>
+      <c r="J187" s="14"/>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A188" s="10"/>
+      <c r="B188" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C188" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D188" s="10">
+        <v>11</v>
+      </c>
+      <c r="E188" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F188" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G188" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H188" s="10"/>
+      <c r="I188" s="10"/>
+      <c r="J188" s="10"/>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A189" s="10"/>
+      <c r="B189" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C189" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D189" s="10">
+        <v>100</v>
+      </c>
+      <c r="E189" s="10"/>
+      <c r="F189" s="10"/>
+      <c r="G189" s="10"/>
+      <c r="H189" s="10"/>
+      <c r="I189" s="10"/>
+      <c r="J189" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A190" s="10"/>
+      <c r="B190" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C190" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D190" s="10">
+        <v>1</v>
+      </c>
+      <c r="E190" s="10"/>
+      <c r="F190" s="10"/>
+      <c r="G190" s="10"/>
+      <c r="H190" s="10"/>
+      <c r="I190" s="10"/>
+      <c r="J190" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A191" s="10"/>
+      <c r="B191" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C191" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D191" s="10">
+        <v>100</v>
+      </c>
+      <c r="E191" s="10"/>
+      <c r="F191" s="10"/>
+      <c r="G191" s="10"/>
+      <c r="H191" s="10"/>
+      <c r="I191" s="10"/>
+      <c r="J191" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A192" s="10"/>
+      <c r="B192" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C192" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D192" s="10"/>
+      <c r="E192" s="10"/>
+      <c r="F192" s="10"/>
+      <c r="G192" s="10"/>
+      <c r="H192" s="10"/>
+      <c r="I192" s="10"/>
+      <c r="J192" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A193" s="10"/>
+      <c r="B193" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C193" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D193" s="10">
+        <v>100</v>
+      </c>
+      <c r="E193" s="10"/>
+      <c r="F193" s="10"/>
+      <c r="G193" s="10"/>
+      <c r="H193" s="10"/>
+      <c r="I193" s="10"/>
+      <c r="J193" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="11"/>
+      <c r="B194" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C194" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D194" s="11"/>
+      <c r="E194" s="11"/>
+      <c r="F194" s="11"/>
+      <c r="G194" s="11"/>
+      <c r="H194" s="11"/>
+      <c r="I194" s="11"/>
+      <c r="J194" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="196" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C196" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G196" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H196" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I196" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J196" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A197" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B197" s="14"/>
+      <c r="C197" s="14"/>
+      <c r="D197" s="14"/>
+      <c r="E197" s="14"/>
+      <c r="F197" s="14"/>
+      <c r="G197" s="14"/>
+      <c r="H197" s="14"/>
+      <c r="I197" s="20"/>
+      <c r="J197" s="14"/>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A198" s="10"/>
+      <c r="B198" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C198" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D198" s="10">
+        <v>11</v>
+      </c>
+      <c r="E198" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F198" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="G198" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="H198" s="10"/>
+      <c r="I198" s="4"/>
+      <c r="J198" s="10"/>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A199" s="10"/>
+      <c r="B199" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C199" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D199" s="10">
+        <v>11</v>
+      </c>
+      <c r="E199" s="10"/>
+      <c r="F199" s="10"/>
+      <c r="G199" s="10"/>
+      <c r="H199" s="10"/>
+      <c r="I199" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J199" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A200" s="10"/>
+      <c r="B200" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C200" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D200" s="10">
+        <v>256</v>
+      </c>
+      <c r="E200" s="10"/>
+      <c r="F200" s="10"/>
+      <c r="G200" s="10"/>
+      <c r="H200" s="10"/>
+      <c r="I200" s="4"/>
+      <c r="J200" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A201" s="10"/>
+      <c r="B201" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C201" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D201" s="10">
+        <v>45</v>
+      </c>
+      <c r="E201" s="10"/>
+      <c r="F201" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G201" s="10"/>
+      <c r="H201" s="10"/>
+      <c r="I201" s="4"/>
+      <c r="J201" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A202" s="10"/>
+      <c r="B202" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C202" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D202" s="10">
+        <v>11</v>
+      </c>
+      <c r="E202" s="10"/>
+      <c r="F202" s="10"/>
+      <c r="G202" s="10"/>
+      <c r="H202" s="10"/>
+      <c r="I202" s="4"/>
+      <c r="J202" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A203" s="10"/>
+      <c r="B203" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C203" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D203" s="10">
+        <v>11</v>
+      </c>
+      <c r="E203" s="10"/>
+      <c r="F203" s="10"/>
+      <c r="G203" s="10"/>
+      <c r="H203" s="10"/>
+      <c r="I203" s="4"/>
+      <c r="J203" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A204" s="10"/>
+      <c r="B204" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C204" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D204" s="10">
+        <v>11</v>
+      </c>
+      <c r="E204" s="10"/>
+      <c r="F204" s="10"/>
+      <c r="G204" s="10"/>
+      <c r="H204" s="10"/>
+      <c r="I204" s="4"/>
+      <c r="J204" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A205" s="10"/>
+      <c r="B205" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C205" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D205" s="10">
+        <v>11</v>
+      </c>
+      <c r="E205" s="10"/>
+      <c r="F205" s="10"/>
+      <c r="G205" s="10"/>
+      <c r="H205" s="10"/>
+      <c r="I205" s="4"/>
+      <c r="J205" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A206" s="10"/>
+      <c r="B206" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="C206" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D206" s="10">
+        <v>11</v>
+      </c>
+      <c r="E206" s="10"/>
+      <c r="F206" s="10"/>
+      <c r="G206" s="10"/>
+      <c r="H206" s="10"/>
+      <c r="I206" s="4"/>
+      <c r="J206" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A207" s="10"/>
+      <c r="B207" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="C207" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D207" s="10">
+        <v>11</v>
+      </c>
+      <c r="E207" s="10"/>
+      <c r="F207" s="10"/>
+      <c r="G207" s="10"/>
+      <c r="H207" s="10"/>
+      <c r="I207" s="4"/>
+      <c r="J207" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A208" s="10"/>
+      <c r="B208" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="C208" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D208" s="10">
+        <v>255</v>
+      </c>
+      <c r="E208" s="10"/>
+      <c r="F208" s="10"/>
+      <c r="G208" s="10"/>
+      <c r="H208" s="10"/>
+      <c r="I208" s="4"/>
+      <c r="J208" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A209" s="10"/>
+      <c r="B209" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="C209" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D209" s="10">
+        <v>255</v>
+      </c>
+      <c r="E209" s="10"/>
+      <c r="F209" s="10"/>
+      <c r="G209" s="10"/>
+      <c r="H209" s="10"/>
+      <c r="I209" s="4"/>
+      <c r="J209" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A210" s="10"/>
+      <c r="B210" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="C210" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D210" s="10">
+        <v>45</v>
+      </c>
+      <c r="E210" s="10"/>
+      <c r="F210" s="10"/>
+      <c r="G210" s="10"/>
+      <c r="H210" s="10"/>
+      <c r="I210" s="4"/>
+      <c r="J210" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A211" s="10"/>
+      <c r="B211" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="C211" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D211" s="10">
+        <v>45</v>
+      </c>
+      <c r="E211" s="10"/>
+      <c r="F211" s="10"/>
+      <c r="G211" s="10"/>
+      <c r="H211" s="10"/>
+      <c r="I211" s="4"/>
+      <c r="J211" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A212" s="10"/>
+      <c r="B212" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="C212" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D212" s="10">
+        <v>45</v>
+      </c>
+      <c r="E212" s="10"/>
+      <c r="F212" s="10"/>
+      <c r="G212" s="10"/>
+      <c r="H212" s="10"/>
+      <c r="I212" s="4"/>
+      <c r="J212" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A213" s="10"/>
+      <c r="B213" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="C213" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D213" s="10">
+        <v>50</v>
+      </c>
+      <c r="E213" s="10"/>
+      <c r="F213" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G213" s="10"/>
+      <c r="H213" s="10"/>
+      <c r="I213" s="4"/>
+      <c r="J213" s="10"/>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A214" s="10"/>
+      <c r="B214" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="C214" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D214" s="10">
+        <v>4</v>
+      </c>
+      <c r="E214" s="10"/>
+      <c r="F214" s="10"/>
+      <c r="G214" s="10"/>
+      <c r="H214" s="10"/>
+      <c r="I214" s="4"/>
+      <c r="J214" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A215" s="10"/>
+      <c r="B215" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="C215" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D215" s="10">
+        <v>11</v>
+      </c>
+      <c r="E215" s="10"/>
+      <c r="F215" s="10"/>
+      <c r="G215" s="10"/>
+      <c r="H215" s="10"/>
+      <c r="I215" s="4"/>
+      <c r="J215" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A216" s="10"/>
+      <c r="B216" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="C216" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D216" s="10">
+        <v>45</v>
+      </c>
+      <c r="E216" s="10"/>
+      <c r="F216" s="10"/>
+      <c r="G216" s="10"/>
+      <c r="H216" s="10"/>
+      <c r="I216" s="4"/>
+      <c r="J216" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A217" s="10"/>
+      <c r="B217" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="C217" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D217" s="10">
+        <v>100</v>
+      </c>
+      <c r="E217" s="10"/>
+      <c r="F217" s="10"/>
+      <c r="G217" s="10"/>
+      <c r="H217" s="10"/>
+      <c r="I217" s="4"/>
+      <c r="J217" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A218" s="10"/>
+      <c r="B218" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="C218" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D218" s="10">
+        <v>4</v>
+      </c>
+      <c r="E218" s="10"/>
+      <c r="F218" s="10"/>
+      <c r="G218" s="10"/>
+      <c r="H218" s="10"/>
+      <c r="I218" s="4"/>
+      <c r="J218" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A219" s="10"/>
+      <c r="B219" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="C219" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D219" s="10">
+        <v>11</v>
+      </c>
+      <c r="E219" s="10"/>
+      <c r="F219" s="10"/>
+      <c r="G219" s="10"/>
+      <c r="H219" s="10"/>
+      <c r="I219" s="4"/>
+      <c r="J219" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A220" s="10"/>
+      <c r="B220" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C220" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D220" s="10">
+        <v>250</v>
+      </c>
+      <c r="E220" s="10"/>
+      <c r="F220" s="10"/>
+      <c r="G220" s="10"/>
+      <c r="H220" s="10"/>
+      <c r="I220" s="4"/>
+      <c r="J220" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A221" s="10"/>
+      <c r="B221" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="C221" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D221" s="10">
+        <v>11</v>
+      </c>
+      <c r="E221" s="10"/>
+      <c r="F221" s="10"/>
+      <c r="G221" s="10"/>
+      <c r="H221" s="10"/>
+      <c r="I221" s="4"/>
+      <c r="J221" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A222" s="10"/>
+      <c r="B222" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="C222" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D222" s="10"/>
+      <c r="E222" s="10"/>
+      <c r="F222" s="10"/>
+      <c r="G222" s="10"/>
+      <c r="H222" s="10"/>
+      <c r="I222" s="4"/>
+      <c r="J222" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A223" s="10"/>
+      <c r="B223" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="C223" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D223" s="10"/>
+      <c r="E223" s="10"/>
+      <c r="F223" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G223" s="10"/>
+      <c r="H223" s="10"/>
+      <c r="I223" s="4"/>
+      <c r="J223" s="10"/>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A224" s="10"/>
+      <c r="B224" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C224" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D224" s="10"/>
+      <c r="E224" s="10"/>
+      <c r="F224" s="10"/>
+      <c r="G224" s="10"/>
+      <c r="H224" s="10"/>
+      <c r="I224" s="4"/>
+      <c r="J224" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A225" s="10"/>
+      <c r="B225" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C225" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D225" s="10"/>
+      <c r="E225" s="10"/>
+      <c r="F225" s="10"/>
+      <c r="G225" s="10"/>
+      <c r="H225" s="10"/>
+      <c r="I225" s="4"/>
+      <c r="J225" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A226" s="10"/>
+      <c r="B226" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C226" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D226" s="10"/>
+      <c r="E226" s="10"/>
+      <c r="F226" s="10"/>
+      <c r="G226" s="10"/>
+      <c r="H226" s="10"/>
+      <c r="I226" s="4"/>
+      <c r="J226" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="11"/>
+      <c r="B227" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="C227" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D227" s="11">
+        <v>50</v>
+      </c>
+      <c r="E227" s="11"/>
+      <c r="F227" s="11"/>
+      <c r="G227" s="11"/>
+      <c r="H227" s="11"/>
+      <c r="I227" s="7"/>
+      <c r="J227" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="5"/>
+      <c r="B228" s="5"/>
+      <c r="C228" s="33"/>
+      <c r="D228" s="5"/>
+      <c r="E228" s="5"/>
+      <c r="F228" s="5"/>
+      <c r="G228" s="5"/>
+      <c r="H228" s="5"/>
+      <c r="I228" s="5"/>
+      <c r="J228" s="5"/>
+    </row>
+    <row r="229" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C229" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F229" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G229" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H229" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I229" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J229" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A230" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B230" s="14"/>
+      <c r="C230" s="14"/>
+      <c r="D230" s="30"/>
+      <c r="E230" s="20"/>
+      <c r="F230" s="14"/>
+      <c r="G230" s="14"/>
+      <c r="H230" s="14"/>
+      <c r="I230" s="14"/>
+      <c r="J230" s="14"/>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A231" s="10"/>
+      <c r="B231" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C231" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D231" s="5">
+        <v>11</v>
+      </c>
+      <c r="E231" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F231" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="G231" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="H231" s="10"/>
+      <c r="I231" s="10"/>
+      <c r="J231" s="10"/>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A232" s="10"/>
+      <c r="B232" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C232" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D232" s="6">
+        <v>11</v>
+      </c>
+      <c r="E232" s="5"/>
+      <c r="F232" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G232" s="10"/>
+      <c r="H232" s="10"/>
+      <c r="I232" s="10"/>
+      <c r="J232" s="10"/>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A233" s="10"/>
+      <c r="B233" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C233" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D233" s="6">
+        <v>11</v>
+      </c>
+      <c r="E233" s="4"/>
+      <c r="F233" s="10"/>
+      <c r="G233" s="10"/>
+      <c r="H233" s="10"/>
+      <c r="I233" s="10"/>
+      <c r="J233" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A234" s="10"/>
+      <c r="B234" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C234" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D234" s="6">
+        <v>45</v>
+      </c>
+      <c r="E234" s="4"/>
+      <c r="F234" s="10"/>
+      <c r="G234" s="10"/>
+      <c r="H234" s="10"/>
+      <c r="I234" s="10"/>
+      <c r="J234" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A235" s="10"/>
+      <c r="B235" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C235" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D235" s="6">
+        <v>45</v>
+      </c>
+      <c r="E235" s="4"/>
+      <c r="F235" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G235" s="10"/>
+      <c r="H235" s="10"/>
+      <c r="I235" s="10"/>
+      <c r="J235" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A236" s="10"/>
+      <c r="B236" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C236" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D236" s="6">
+        <v>45</v>
+      </c>
+      <c r="E236" s="4"/>
+      <c r="F236" s="10"/>
+      <c r="G236" s="10"/>
+      <c r="H236" s="10"/>
+      <c r="I236" s="10"/>
+      <c r="J236" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A237" s="10"/>
+      <c r="B237" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="C237" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D237" s="6">
+        <v>255</v>
+      </c>
+      <c r="E237" s="4"/>
+      <c r="F237" s="10"/>
+      <c r="G237" s="10"/>
+      <c r="H237" s="10"/>
+      <c r="I237" s="10"/>
+      <c r="J237" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A238" s="10"/>
+      <c r="B238" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="C238" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D238" s="6">
+        <v>255</v>
+      </c>
+      <c r="E238" s="4"/>
+      <c r="F238" s="10"/>
+      <c r="G238" s="10"/>
+      <c r="H238" s="10"/>
+      <c r="I238" s="10"/>
+      <c r="J238" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A239" s="10"/>
+      <c r="B239" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="C239" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D239" s="6">
+        <v>45</v>
+      </c>
+      <c r="E239" s="4"/>
+      <c r="F239" s="10"/>
+      <c r="G239" s="10"/>
+      <c r="H239" s="10"/>
+      <c r="I239" s="10"/>
+      <c r="J239" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A240" s="10"/>
+      <c r="B240" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="C240" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D240" s="6">
+        <v>45</v>
+      </c>
+      <c r="E240" s="4"/>
+      <c r="F240" s="10"/>
+      <c r="G240" s="10"/>
+      <c r="H240" s="10"/>
+      <c r="I240" s="10"/>
+      <c r="J240" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A241" s="10"/>
+      <c r="B241" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="C241" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D241" s="6">
+        <v>45</v>
+      </c>
+      <c r="E241" s="4"/>
+      <c r="F241" s="10"/>
+      <c r="G241" s="10"/>
+      <c r="H241" s="10"/>
+      <c r="I241" s="10"/>
+      <c r="J241" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A242" s="10"/>
+      <c r="B242" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="C242" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D242" s="6">
+        <v>50</v>
+      </c>
+      <c r="E242" s="4"/>
+      <c r="F242" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G242" s="10"/>
+      <c r="H242" s="10"/>
+      <c r="I242" s="10"/>
+      <c r="J242" s="10"/>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A243" s="10"/>
+      <c r="B243" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="C243" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D243" s="6">
+        <v>4</v>
+      </c>
+      <c r="E243" s="4"/>
+      <c r="F243" s="10"/>
+      <c r="G243" s="10"/>
+      <c r="H243" s="10"/>
+      <c r="I243" s="10"/>
+      <c r="J243" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A244" s="10"/>
+      <c r="B244" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="C244" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D244" s="6">
+        <v>11</v>
+      </c>
+      <c r="E244" s="4"/>
+      <c r="F244" s="10"/>
+      <c r="G244" s="10"/>
+      <c r="H244" s="10"/>
+      <c r="I244" s="10"/>
+      <c r="J244" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A245" s="10"/>
+      <c r="B245" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="C245" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D245" s="6">
+        <v>45</v>
+      </c>
+      <c r="E245" s="4"/>
+      <c r="F245" s="10"/>
+      <c r="G245" s="10"/>
+      <c r="H245" s="10"/>
+      <c r="I245" s="10"/>
+      <c r="J245" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A246" s="10"/>
+      <c r="B246" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="C246" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D246" s="6">
+        <v>250</v>
+      </c>
+      <c r="E246" s="4"/>
+      <c r="F246" s="10"/>
+      <c r="G246" s="10"/>
+      <c r="H246" s="10"/>
+      <c r="I246" s="10"/>
+      <c r="J246" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A247" s="10"/>
+      <c r="B247" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="C247" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D247" s="6">
+        <v>4</v>
+      </c>
+      <c r="E247" s="4"/>
+      <c r="F247" s="10"/>
+      <c r="G247" s="10"/>
+      <c r="H247" s="10"/>
+      <c r="I247" s="10"/>
+      <c r="J247" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A248" s="10"/>
+      <c r="B248" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="C248" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D248" s="6">
+        <v>11</v>
+      </c>
+      <c r="E248" s="4"/>
+      <c r="F248" s="10"/>
+      <c r="G248" s="10"/>
+      <c r="H248" s="10"/>
+      <c r="I248" s="10"/>
+      <c r="J248" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A249" s="10"/>
+      <c r="B249" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C249" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D249" s="6">
+        <v>250</v>
+      </c>
+      <c r="E249" s="4"/>
+      <c r="F249" s="10"/>
+      <c r="G249" s="10"/>
+      <c r="H249" s="10"/>
+      <c r="I249" s="10"/>
+      <c r="J249" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A250" s="10"/>
+      <c r="B250" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="C250" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D250" s="6">
+        <v>11</v>
+      </c>
+      <c r="E250" s="4"/>
+      <c r="F250" s="10"/>
+      <c r="G250" s="10"/>
+      <c r="H250" s="10"/>
+      <c r="I250" s="10"/>
+      <c r="J250" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A251" s="10"/>
+      <c r="B251" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="C251" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D251" s="6"/>
+      <c r="E251" s="4"/>
+      <c r="F251" s="10"/>
+      <c r="G251" s="10"/>
+      <c r="H251" s="10"/>
+      <c r="I251" s="10"/>
+      <c r="J251" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A252" s="10"/>
+      <c r="B252" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="C252" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D252" s="6"/>
+      <c r="E252" s="4"/>
+      <c r="F252" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G252" s="10"/>
+      <c r="H252" s="10"/>
+      <c r="I252" s="10"/>
+      <c r="J252" s="10"/>
+    </row>
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A253" s="10"/>
+      <c r="B253" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C253" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D253" s="6"/>
+      <c r="E253" s="4"/>
+      <c r="F253" s="10"/>
+      <c r="G253" s="10"/>
+      <c r="H253" s="10"/>
+      <c r="I253" s="10"/>
+      <c r="J253" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A254" s="10"/>
+      <c r="B254" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C254" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D254" s="6"/>
+      <c r="E254" s="4"/>
+      <c r="F254" s="10"/>
+      <c r="G254" s="10"/>
+      <c r="H254" s="10"/>
+      <c r="I254" s="10"/>
+      <c r="J254" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A255" s="10"/>
+      <c r="B255" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C255" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D255" s="6"/>
+      <c r="E255" s="4"/>
+      <c r="F255" s="10"/>
+      <c r="G255" s="10"/>
+      <c r="H255" s="10"/>
+      <c r="I255" s="10"/>
+      <c r="J255" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A256" s="11"/>
+      <c r="B256" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="C256" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D256" s="9">
+        <v>50</v>
+      </c>
+      <c r="E256" s="7"/>
+      <c r="F256" s="11"/>
+      <c r="G256" s="11"/>
+      <c r="H256" s="11"/>
+      <c r="I256" s="11"/>
+      <c r="J256" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A257" s="5"/>
+      <c r="B257" s="5"/>
+      <c r="C257" s="5"/>
+      <c r="D257" s="5"/>
+      <c r="E257" s="5"/>
+      <c r="F257" s="5"/>
+      <c r="G257" s="5"/>
+      <c r="H257" s="5"/>
+      <c r="I257" s="5"/>
+      <c r="J257" s="33"/>
+    </row>
+    <row r="259" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="260" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A260" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B260" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D260" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F260" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G260" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H260" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I260" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J260" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A261" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B261" s="10"/>
+      <c r="C261" s="10"/>
+      <c r="D261" s="6"/>
+      <c r="E261" s="10"/>
+      <c r="F261" s="10"/>
+      <c r="G261" s="10"/>
+      <c r="H261" s="10"/>
+      <c r="I261" s="10"/>
+      <c r="J261" s="10"/>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A262" s="4"/>
+      <c r="B262" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C262" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D262" s="6">
+        <v>11</v>
+      </c>
+      <c r="E262" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F262" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G262" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H262" s="10"/>
+      <c r="I262" s="10"/>
+      <c r="J262" s="10"/>
+    </row>
+    <row r="263" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A263" s="4"/>
+      <c r="B263" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C263" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D263" s="6">
+        <v>11</v>
+      </c>
+      <c r="E263" s="10"/>
+      <c r="F263" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G263" s="10"/>
+      <c r="H263" s="10"/>
+      <c r="I263" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J263" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A264" s="7"/>
+      <c r="B264" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C264" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D264" s="9">
+        <v>11</v>
+      </c>
+      <c r="E264" s="11"/>
+      <c r="F264" s="11"/>
+      <c r="G264" s="11"/>
+      <c r="H264" s="11"/>
+      <c r="I264" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J264" s="11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A265" s="5"/>
+      <c r="B265" s="5"/>
+      <c r="C265" s="5"/>
+      <c r="D265" s="5"/>
+      <c r="E265" s="5"/>
+      <c r="F265" s="5"/>
+      <c r="G265" s="5"/>
+      <c r="H265" s="5"/>
+      <c r="I265" s="5"/>
+      <c r="J265" s="33"/>
+    </row>
+    <row r="267" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="268" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A268" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="B268" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D268" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F268" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G268" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H268" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I268" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J268" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A269" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="B269" s="10"/>
+      <c r="C269" s="10"/>
+      <c r="D269" s="6"/>
+      <c r="E269" s="10"/>
+      <c r="F269" s="10"/>
+      <c r="G269" s="10"/>
+      <c r="H269" s="10"/>
+      <c r="I269" s="10"/>
+      <c r="J269" s="10"/>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A270" s="4"/>
+      <c r="B270" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C270" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D270" s="6">
+        <v>11</v>
+      </c>
+      <c r="E270" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F270" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G270" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H270" s="10"/>
+      <c r="I270" s="10"/>
+      <c r="J270" s="10"/>
+    </row>
+    <row r="271" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A271" s="4"/>
+      <c r="B271" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C271" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D271" s="6">
+        <v>11</v>
+      </c>
+      <c r="E271" s="10"/>
+      <c r="F271" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G271" s="10"/>
+      <c r="H271" s="10"/>
+      <c r="I271" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J271" s="11"/>
+    </row>
+    <row r="272" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A272" s="7"/>
+      <c r="B272" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C272" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D272" s="9">
+        <v>11</v>
+      </c>
+      <c r="E272" s="11"/>
+      <c r="F272" s="11"/>
+      <c r="G272" s="11"/>
+      <c r="H272" s="11"/>
+      <c r="I272" s="11"/>
+      <c r="J272" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="274" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A274" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F274" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G274" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H274" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I274" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J274" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A275" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="B275" s="10"/>
+      <c r="C275" s="10"/>
+      <c r="D275" s="35"/>
+      <c r="E275" s="10"/>
+      <c r="F275" s="10"/>
+      <c r="G275" s="10"/>
+      <c r="H275" s="10"/>
+      <c r="I275" s="10"/>
+      <c r="J275" s="6"/>
+    </row>
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A276" s="4"/>
+      <c r="B276" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C276" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D276" s="35">
+        <v>11</v>
+      </c>
+      <c r="E276" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F276" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G276" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H276" s="10"/>
+      <c r="I276" s="10"/>
+      <c r="J276" s="6"/>
+    </row>
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A277" s="4"/>
+      <c r="B277" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C277" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D277" s="35">
+        <v>255</v>
+      </c>
+      <c r="E277" s="10"/>
+      <c r="F277" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G277" s="10"/>
+      <c r="H277" s="10"/>
+      <c r="I277" s="10"/>
+      <c r="J277" s="6"/>
+    </row>
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A278" s="4"/>
+      <c r="B278" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C278" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D278" s="35">
+        <v>255</v>
+      </c>
+      <c r="E278" s="10"/>
+      <c r="F278" s="10"/>
+      <c r="G278" s="10"/>
+      <c r="H278" s="10"/>
+      <c r="I278" s="10"/>
+      <c r="J278" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A279" s="4"/>
+      <c r="B279" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C279" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D279" s="35">
+        <v>255</v>
+      </c>
+      <c r="E279" s="10"/>
+      <c r="F279" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G279" s="10"/>
+      <c r="H279" s="10"/>
+      <c r="I279" s="10"/>
+      <c r="J279" s="6"/>
+    </row>
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A280" s="4"/>
+      <c r="B280" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C280" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D280" s="35">
+        <v>255</v>
+      </c>
+      <c r="E280" s="10"/>
+      <c r="F280" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G280" s="10"/>
+      <c r="H280" s="10"/>
+      <c r="I280" s="10"/>
+      <c r="J280" s="6"/>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A281" s="4"/>
+      <c r="B281" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C281" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D281" s="35">
+        <v>255</v>
+      </c>
+      <c r="E281" s="10"/>
+      <c r="F281" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G281" s="10"/>
+      <c r="H281" s="10"/>
+      <c r="I281" s="10"/>
+      <c r="J281" s="6"/>
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A282" s="4"/>
+      <c r="B282" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C282" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D282" s="35">
+        <v>11</v>
+      </c>
+      <c r="E282" s="10"/>
+      <c r="F282" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G282" s="10"/>
+      <c r="H282" s="10"/>
+      <c r="I282" s="10"/>
+      <c r="J282" s="6"/>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A283" s="4"/>
+      <c r="B283" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C283" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D283" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="E283" s="10"/>
+      <c r="F283" s="10"/>
+      <c r="G283" s="10"/>
+      <c r="H283" s="10"/>
+      <c r="I283" s="10"/>
+      <c r="J283" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A284" s="4"/>
+      <c r="B284" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C284" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D284" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="E284" s="10"/>
+      <c r="F284" s="10"/>
+      <c r="G284" s="10"/>
+      <c r="H284" s="10"/>
+      <c r="I284" s="10"/>
+      <c r="J284" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A285" s="4"/>
+      <c r="B285" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C285" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D285" s="18">
+        <v>100</v>
+      </c>
+      <c r="E285" s="10"/>
+      <c r="F285" s="10"/>
+      <c r="G285" s="10"/>
+      <c r="H285" s="10"/>
+      <c r="I285" s="10"/>
+      <c r="J285" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A286" s="4"/>
+      <c r="B286" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C286" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D286" s="10"/>
+      <c r="E286" s="10"/>
+      <c r="F286" s="10"/>
+      <c r="G286" s="10"/>
+      <c r="H286" s="10"/>
+      <c r="I286" s="10"/>
+      <c r="J286" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A287" s="4"/>
+      <c r="B287" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C287" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D287" s="10">
+        <v>100</v>
+      </c>
+      <c r="E287" s="10"/>
+      <c r="F287" s="10"/>
+      <c r="G287" s="10"/>
+      <c r="H287" s="10"/>
+      <c r="I287" s="10"/>
+      <c r="J287" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A288" s="4"/>
+      <c r="B288" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C288" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D288" s="10"/>
+      <c r="E288" s="10"/>
+      <c r="F288" s="10"/>
+      <c r="G288" s="10"/>
+      <c r="H288" s="10"/>
+      <c r="I288" s="10"/>
+      <c r="J288" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A289" s="7"/>
+      <c r="B289" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C289" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D289" s="11">
+        <v>11</v>
+      </c>
+      <c r="E289" s="11"/>
+      <c r="F289" s="11"/>
+      <c r="G289" s="11"/>
+      <c r="H289" s="11"/>
+      <c r="I289" s="11"/>
+      <c r="J289" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="290" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="291" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A291" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F291" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G291" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H291" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I291" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J291" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A292" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B292" s="10"/>
+      <c r="C292" s="10"/>
+      <c r="D292" s="35"/>
+      <c r="E292" s="10"/>
+      <c r="F292" s="10"/>
+      <c r="G292" s="10"/>
+      <c r="H292" s="10"/>
+      <c r="I292" s="10"/>
+      <c r="J292" s="6"/>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A293" s="4"/>
+      <c r="B293" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C293" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D293" s="35">
+        <v>11</v>
+      </c>
+      <c r="E293" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F293" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G293" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H293" s="10"/>
+      <c r="I293" s="10"/>
+      <c r="J293" s="6"/>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A294" s="4"/>
+      <c r="B294" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C294" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D294" s="35">
+        <v>11</v>
+      </c>
+      <c r="E294" s="10"/>
+      <c r="F294" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G294" s="10"/>
+      <c r="H294" s="10"/>
+      <c r="I294" s="10"/>
+      <c r="J294" s="6"/>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A295" s="4"/>
+      <c r="B295" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C295" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D295" s="35">
+        <v>11</v>
+      </c>
+      <c r="E295" s="10"/>
+      <c r="F295" s="10"/>
+      <c r="G295" s="10"/>
+      <c r="H295" s="10"/>
+      <c r="I295" s="10"/>
+      <c r="J295" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A296" s="4"/>
+      <c r="B296" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="C296" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D296" s="35">
+        <v>11</v>
+      </c>
+      <c r="E296" s="10"/>
+      <c r="F296" s="10"/>
+      <c r="G296" s="10"/>
+      <c r="H296" s="10"/>
+      <c r="I296" s="10"/>
+      <c r="J296" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A297" s="4"/>
+      <c r="B297" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C297" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D297" s="35">
+        <v>11</v>
+      </c>
+      <c r="E297" s="10"/>
+      <c r="F297" s="10"/>
+      <c r="G297" s="10"/>
+      <c r="H297" s="10"/>
+      <c r="I297" s="10"/>
+      <c r="J297" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A298" s="4"/>
+      <c r="B298" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C298" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D298" s="35">
+        <v>45</v>
+      </c>
+      <c r="E298" s="10"/>
+      <c r="F298" s="10"/>
+      <c r="G298" s="10"/>
+      <c r="H298" s="10"/>
+      <c r="I298" s="10"/>
+      <c r="J298" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A299" s="4"/>
+      <c r="B299" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C299" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D299" s="35">
+        <v>255</v>
+      </c>
+      <c r="E299" s="10"/>
+      <c r="F299" s="10"/>
+      <c r="G299" s="10"/>
+      <c r="H299" s="10"/>
+      <c r="I299" s="10"/>
+      <c r="J299" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A300" s="4"/>
+      <c r="B300" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C300" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D300" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="E300" s="10"/>
+      <c r="F300" s="10"/>
+      <c r="G300" s="10"/>
+      <c r="H300" s="10"/>
+      <c r="I300" s="10"/>
+      <c r="J300" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A301" s="4"/>
+      <c r="B301" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C301" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D301" s="18">
+        <v>100</v>
+      </c>
+      <c r="E301" s="10"/>
+      <c r="F301" s="10"/>
+      <c r="G301" s="10"/>
+      <c r="H301" s="10"/>
+      <c r="I301" s="10"/>
+      <c r="J301" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A302" s="4"/>
+      <c r="B302" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C302" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D302" s="10"/>
+      <c r="E302" s="10"/>
+      <c r="F302" s="10"/>
+      <c r="G302" s="10"/>
+      <c r="H302" s="10"/>
+      <c r="I302" s="10"/>
+      <c r="J302" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A303" s="4"/>
+      <c r="B303" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C303" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D303" s="10">
+        <v>100</v>
+      </c>
+      <c r="E303" s="10"/>
+      <c r="F303" s="10"/>
+      <c r="G303" s="10"/>
+      <c r="H303" s="10"/>
+      <c r="I303" s="10"/>
+      <c r="J303" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A304" s="7"/>
+      <c r="B304" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C304" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D304" s="11"/>
+      <c r="E304" s="11"/>
+      <c r="F304" s="11"/>
+      <c r="G304" s="11"/>
+      <c r="H304" s="11"/>
+      <c r="I304" s="11"/>
+      <c r="J304" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A305" s="4"/>
+      <c r="B305"/>
+      <c r="C305"/>
+      <c r="D305"/>
+      <c r="E305"/>
+      <c r="F305"/>
+      <c r="G305"/>
+      <c r="H305"/>
+      <c r="I305"/>
+      <c r="J305"/>
+    </row>
+    <row r="306" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A306" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B306" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C306" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D306" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E306" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F306" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G306" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H306" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I306" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J306" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A307" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="B307" s="14"/>
+      <c r="C307" s="14"/>
+      <c r="D307" s="14"/>
+      <c r="E307" s="14"/>
+      <c r="F307" s="14"/>
+      <c r="G307" s="14"/>
+      <c r="H307" s="14"/>
+      <c r="I307" s="14"/>
+      <c r="J307" s="14"/>
+    </row>
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A308" s="10"/>
+      <c r="B308" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C308" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D308" s="10">
+        <v>11</v>
+      </c>
+      <c r="E308" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F308" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G308" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H308" s="10"/>
+      <c r="I308" s="10"/>
+      <c r="J308" s="10"/>
+    </row>
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A309" s="10"/>
+      <c r="B309" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C309" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D309" s="10">
+        <v>11</v>
+      </c>
+      <c r="E309" s="10"/>
+      <c r="F309" s="10"/>
+      <c r="G309" s="10"/>
+      <c r="H309" s="10"/>
+      <c r="I309" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J309" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A310" s="10"/>
+      <c r="B310" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="C310" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D310" s="10">
+        <v>10</v>
+      </c>
+      <c r="E310" s="10"/>
+      <c r="F310" s="10"/>
+      <c r="G310" s="10"/>
+      <c r="H310" s="10"/>
+      <c r="I310" s="10"/>
+      <c r="J310" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A311" s="10"/>
+      <c r="B311" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C311" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D311" s="10">
+        <v>250</v>
+      </c>
+      <c r="E311" s="10"/>
+      <c r="F311" s="10"/>
+      <c r="G311" s="10"/>
+      <c r="H311" s="10"/>
+      <c r="I311" s="10"/>
+      <c r="J311" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A312" s="10"/>
+      <c r="B312" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C312" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D312" s="10">
+        <v>11</v>
+      </c>
+      <c r="E312" s="10"/>
+      <c r="F312" s="10"/>
+      <c r="G312" s="10"/>
+      <c r="H312" s="10"/>
+      <c r="I312" s="10"/>
+      <c r="J312" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A313" s="10"/>
+      <c r="B313" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C313" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D313" s="10">
+        <v>1</v>
+      </c>
+      <c r="E313" s="10"/>
+      <c r="F313" s="10"/>
+      <c r="G313" s="10"/>
+      <c r="H313" s="10"/>
+      <c r="I313" s="10"/>
+      <c r="J313" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A314" s="10"/>
+      <c r="B314" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C314" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D314" s="10">
+        <v>100</v>
+      </c>
+      <c r="E314" s="10"/>
+      <c r="F314" s="10"/>
+      <c r="G314" s="10"/>
+      <c r="H314" s="10"/>
+      <c r="I314" s="10"/>
+      <c r="J314" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A315" s="10"/>
+      <c r="B315" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C315" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D315" s="10"/>
+      <c r="E315" s="10"/>
+      <c r="F315" s="10"/>
+      <c r="G315" s="10"/>
+      <c r="H315" s="10"/>
+      <c r="I315" s="10"/>
+      <c r="J315" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A316" s="10"/>
+      <c r="B316" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C316" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D316" s="10">
+        <v>100</v>
+      </c>
+      <c r="E316" s="10"/>
+      <c r="F316" s="10"/>
+      <c r="G316" s="10"/>
+      <c r="H316" s="10"/>
+      <c r="I316" s="10"/>
+      <c r="J316" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="317" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A317" s="11"/>
+      <c r="B317" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C317" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D317" s="11"/>
+      <c r="E317" s="11"/>
+      <c r="F317" s="11"/>
+      <c r="G317" s="11"/>
+      <c r="H317" s="11"/>
+      <c r="I317" s="11"/>
+      <c r="J317" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4696,10 +7467,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -4729,7 +7500,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
-      <c r="B2" s="25"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -4741,7 +7512,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="24" t="s">
         <v>120</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -4761,7 +7532,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>72</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -4783,7 +7554,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>121</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -4803,7 +7574,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>122</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -4825,7 +7596,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>123</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -4845,7 +7616,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>124</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -4863,7 +7634,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>125</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -4883,7 +7654,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="24" t="s">
         <v>126</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -4905,7 +7676,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>127</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -4925,7 +7696,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -4945,7 +7716,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -4963,7 +7734,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -4983,7 +7754,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="24" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -5001,7 +7772,7 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="25" t="s">
         <v>128</v>
       </c>
       <c r="C16" s="11" t="s">

</xml_diff>